<commit_message>
final changes to new fork
</commit_message>
<xml_diff>
--- a/Theoretical Part/excels/AVL tree time experiment.xlsx
+++ b/Theoretical Part/excels/AVL tree time experiment.xlsx
@@ -14,7 +14,10 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3" uniqueCount="3">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4" uniqueCount="4">
+  <si>
+    <t>Unnamed: 0</t>
+  </si>
   <si>
     <t>Start</t>
   </si>
@@ -380,13 +383,13 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:D11"/>
+  <dimension ref="A1:E11"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <sheetData>
-    <row r="1" spans="1:4">
+    <row r="1" spans="1:5">
       <c r="B1" s="1" t="s">
         <v>0</v>
       </c>
@@ -396,145 +399,178 @@
       <c r="D1" s="1" t="s">
         <v>2</v>
       </c>
-    </row>
-    <row r="2" spans="1:4">
+      <c r="E1" s="1" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="2" spans="1:5">
       <c r="A2" s="1">
         <v>0</v>
       </c>
       <c r="B2">
-        <v>0.1135909999998148</v>
+        <v>0</v>
       </c>
       <c r="C2">
-        <v>0.1239215999999033</v>
+        <v>7.572733333320986E-05</v>
       </c>
       <c r="D2">
-        <v>0.1305323999999928</v>
-      </c>
-    </row>
-    <row r="3" spans="1:4">
+        <v>8.261439999993554E-05</v>
+      </c>
+      <c r="E2">
+        <v>8.70215999999952E-05</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5">
       <c r="A3" s="1">
         <v>1</v>
       </c>
       <c r="B3">
-        <v>0.234311899999966</v>
+        <v>1</v>
       </c>
       <c r="C3">
-        <v>0.2612277999999151</v>
+        <v>7.810396666665533E-05</v>
       </c>
       <c r="D3">
-        <v>0.2636159999999563</v>
-      </c>
-    </row>
-    <row r="4" spans="1:4">
+        <v>8.707593333330503E-05</v>
+      </c>
+      <c r="E3">
+        <v>8.787199999998542E-05</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5">
       <c r="A4" s="1">
         <v>2</v>
       </c>
       <c r="B4">
-        <v>0.3620896999998422</v>
+        <v>2</v>
       </c>
       <c r="C4">
-        <v>0.3937186000000565</v>
+        <v>8.046437777774272E-05</v>
       </c>
       <c r="D4">
-        <v>0.4150615999999445</v>
-      </c>
-    </row>
-    <row r="5" spans="1:4">
+        <v>8.749302222223478E-05</v>
+      </c>
+      <c r="E4">
+        <v>9.223591111109879E-05</v>
+      </c>
+    </row>
+    <row r="5" spans="1:5">
       <c r="A5" s="1">
         <v>3</v>
       </c>
       <c r="B5">
-        <v>0.5038150000000314</v>
+        <v>3</v>
       </c>
       <c r="C5">
-        <v>0.538168799999994</v>
+        <v>8.39691666666719E-05</v>
       </c>
       <c r="D5">
-        <v>0.552687399999968</v>
-      </c>
-    </row>
-    <row r="6" spans="1:4">
+        <v>8.9694799999999E-05</v>
+      </c>
+      <c r="E5">
+        <v>9.211456666666133E-05</v>
+      </c>
+    </row>
+    <row r="6" spans="1:5">
       <c r="A6" s="1">
         <v>4</v>
       </c>
       <c r="B6">
-        <v>0.6359192999998413</v>
+        <v>4</v>
       </c>
       <c r="C6">
-        <v>0.6879839000000629</v>
+        <v>8.478923999997884E-05</v>
       </c>
       <c r="D6">
-        <v>0.7238902000001417</v>
-      </c>
-    </row>
-    <row r="7" spans="1:4">
+        <v>9.173118666667506E-05</v>
+      </c>
+      <c r="E6">
+        <v>9.651869333335222E-05</v>
+      </c>
+    </row>
+    <row r="7" spans="1:5">
       <c r="A7" s="1">
         <v>5</v>
       </c>
       <c r="B7">
-        <v>0.7591620000000603</v>
+        <v>5</v>
       </c>
       <c r="C7">
-        <v>0.8267794000000777</v>
+        <v>8.435133333334004E-05</v>
       </c>
       <c r="D7">
-        <v>0.824934600000006</v>
-      </c>
-    </row>
-    <row r="8" spans="1:4">
+        <v>9.18643777777864E-05</v>
+      </c>
+      <c r="E7">
+        <v>9.165940000000066E-05</v>
+      </c>
+    </row>
+    <row r="8" spans="1:5">
       <c r="A8" s="1">
         <v>6</v>
       </c>
       <c r="B8">
-        <v>0.8940727000001516</v>
+        <v>6</v>
       </c>
       <c r="C8">
-        <v>1.000173000000132</v>
+        <v>8.51497809523954E-05</v>
       </c>
       <c r="D8">
-        <v>1.017483999999968</v>
-      </c>
-    </row>
-    <row r="9" spans="1:4">
+        <v>9.525457142858401E-05</v>
+      </c>
+      <c r="E8">
+        <v>9.690323809523506E-05</v>
+      </c>
+    </row>
+    <row r="9" spans="1:5">
       <c r="A9" s="1">
         <v>7</v>
       </c>
       <c r="B9">
-        <v>1.036931299999878</v>
+        <v>7</v>
       </c>
       <c r="C9">
-        <v>1.170208699999876</v>
+        <v>8.641094166665651E-05</v>
       </c>
       <c r="D9">
-        <v>1.222927700000128</v>
-      </c>
-    </row>
-    <row r="10" spans="1:4">
+        <v>9.751739166665634E-05</v>
+      </c>
+      <c r="E9">
+        <v>0.0001019106416666773</v>
+      </c>
+    </row>
+    <row r="10" spans="1:5">
       <c r="A10" s="1">
         <v>8</v>
       </c>
       <c r="B10">
-        <v>1.280333100000007</v>
+        <v>8</v>
       </c>
       <c r="C10">
-        <v>1.590719499999977</v>
+        <v>9.483948888888942E-05</v>
       </c>
       <c r="D10">
-        <v>1.572161499999993</v>
-      </c>
-    </row>
-    <row r="11" spans="1:4">
+        <v>0.0001178310740740724</v>
+      </c>
+      <c r="E10">
+        <v>0.0001164564074074069</v>
+      </c>
+    </row>
+    <row r="11" spans="1:5">
       <c r="A11" s="1">
         <v>9</v>
       </c>
       <c r="B11">
-        <v>1.514331500000026</v>
+        <v>9</v>
       </c>
       <c r="C11">
-        <v>1.550628299999971</v>
+        <v>0.0001009554333333351</v>
       </c>
       <c r="D11">
-        <v>1.624247200000127</v>
+        <v>0.0001033752199999981</v>
+      </c>
+      <c r="E11">
+        <v>0.0001082831466666751</v>
       </c>
     </row>
   </sheetData>

</xml_diff>